<commit_message>
Específicos , commit parcial
</commit_message>
<xml_diff>
--- a/log/tabelas resumo.xlsx
+++ b/log/tabelas resumo.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Classicos" sheetId="1" r:id="rId1"/>
+    <sheet name="Correcao" sheetId="3" r:id="rId2"/>
+    <sheet name="Específicos" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="29">
   <si>
     <t>Estratégia</t>
   </si>
@@ -63,9 +65,6 @@
     <t>A-n80-k10</t>
   </si>
   <si>
-    <t>Fitness Ótimo</t>
-  </si>
-  <si>
     <t>2 Pontos</t>
   </si>
   <si>
@@ -79,13 +78,54 @@
   </si>
   <si>
     <t>Geração Melhor</t>
+  </si>
+  <si>
+    <t>Variação</t>
+  </si>
+  <si>
+    <t>Fitness Referência</t>
+  </si>
+  <si>
+    <t>REFAZER TABELA DEPOIS DOS ESPECIFICOS!!!!</t>
+  </si>
+  <si>
+    <t>PMX</t>
+  </si>
+  <si>
+    <t>Melhor Rodada 1</t>
+  </si>
+  <si>
+    <t>Melhor Rodada 2</t>
+  </si>
+  <si>
+    <t>Melhor Rodada 3</t>
+  </si>
+  <si>
+    <t>Pior Fitness</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>SRM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -118,7 +158,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,8 +171,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -149,47 +195,211 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="15">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+  <cellStyles count="65">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -518,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N4" sqref="A4:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -529,7 +739,7 @@
     <col min="12" max="12" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="30">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="30">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -537,10 +747,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -567,16 +777,19 @@
         <v>8</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>1</v>
       </c>
@@ -597,7 +810,7 @@
         <v>500</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -611,7 +824,7 @@
         <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L2">
         <f>F2+H2+I2+J2</f>
@@ -626,8 +839,12 @@
       <c r="O2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="Q2" s="3">
+        <f t="shared" ref="Q2:Q3" si="0">(N2-C2)/C2</f>
+        <v>183.07044553706504</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>2</v>
       </c>
@@ -644,28 +861,28 @@
         <v>10000</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F6" si="0">E3/2</f>
+        <f t="shared" ref="F3:F6" si="1">E3/2</f>
         <v>5000</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I6" si="1">E3*0.4 -H3</f>
+        <f t="shared" ref="I3:I6" si="2">E3*0.4 -H3</f>
         <v>4000</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J6" si="2">E3*0.1</f>
+        <f t="shared" ref="J3:J6" si="3">E3*0.1</f>
         <v>1000</v>
       </c>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L6" si="3">F3+H3+I3+J3</f>
+        <f t="shared" ref="L3:L6" si="4">F3+H3+I3+J3</f>
         <v>10000</v>
       </c>
       <c r="M3">
@@ -677,8 +894,12 @@
       <c r="O3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="Q3" s="3">
+        <f t="shared" si="0"/>
+        <v>1.8555046898638425</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>3</v>
       </c>
@@ -695,28 +916,28 @@
         <v>1000</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>400</v>
       </c>
       <c r="J4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1000</v>
       </c>
       <c r="M4">
@@ -728,8 +949,12 @@
       <c r="O4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="Q4" s="3">
+        <f>(N4-C4)/C4</f>
+        <v>0.88946777251184839</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>4</v>
       </c>
@@ -746,28 +971,28 @@
         <v>1000</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>399</v>
       </c>
       <c r="J5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="K5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1000</v>
       </c>
       <c r="M5">
@@ -779,8 +1004,12 @@
       <c r="O5">
         <v>94</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="Q5" s="3">
+        <f t="shared" ref="Q5:Q6" si="5">(N5-C5)/C5</f>
+        <v>1.2648131677018635</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>5</v>
       </c>
@@ -797,28 +1026,28 @@
         <v>10000</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5000</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4000</v>
       </c>
       <c r="J6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1000</v>
       </c>
       <c r="K6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10000</v>
       </c>
       <c r="M6">
@@ -829,6 +1058,1040 @@
       </c>
       <c r="O6">
         <v>1</v>
+      </c>
+      <c r="Q6" s="3">
+        <f t="shared" si="5"/>
+        <v>410.1134484126984</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="12" max="12" width="13.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="30">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>661</v>
+      </c>
+      <c r="D2">
+        <v>10000</v>
+      </c>
+      <c r="E2">
+        <v>1000</v>
+      </c>
+      <c r="F2">
+        <f>E2/2</f>
+        <v>500</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>E2*0.4 -H2</f>
+        <v>400</v>
+      </c>
+      <c r="J2">
+        <f>E2*0.1</f>
+        <v>100</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2">
+        <f>F2+H2+I2+J2</f>
+        <v>1000</v>
+      </c>
+      <c r="Q2" s="3">
+        <f t="shared" ref="Q2:Q3" si="0">(N2-C2)/C2</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>661</v>
+      </c>
+      <c r="D3">
+        <v>10000</v>
+      </c>
+      <c r="E3">
+        <v>10000</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F6" si="1">E3/2</f>
+        <v>5000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I6" si="2">E3*0.4 -H3</f>
+        <v>4000</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J6" si="3">E3*0.1</f>
+        <v>1000</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L6" si="4">F3+H3+I3+J3</f>
+        <v>10000</v>
+      </c>
+      <c r="Q3" s="3">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>211</v>
+      </c>
+      <c r="D4">
+        <v>10000</v>
+      </c>
+      <c r="E4">
+        <v>1000</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>400</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="Q4" s="3">
+        <f>(N4-C4)/C4</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>805</v>
+      </c>
+      <c r="D5">
+        <v>10000</v>
+      </c>
+      <c r="E5">
+        <v>1000</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>399</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="Q5" s="3">
+        <f t="shared" ref="Q5:Q6" si="5">(N5-C5)/C5</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>1764</v>
+      </c>
+      <c r="D6">
+        <v>10000</v>
+      </c>
+      <c r="E6">
+        <v>10000</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>4000</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>1000</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>10000</v>
+      </c>
+      <c r="Q6" s="3">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="30">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>661</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="5">
+        <f>E2* 0.3</f>
+        <v>300</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5">
+        <f>E2*0.3 -H2</f>
+        <v>299</v>
+      </c>
+      <c r="J2" s="5">
+        <f>E2*0.4</f>
+        <v>400</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="5">
+        <f>F2+H2+I2+J2</f>
+        <v>1000</v>
+      </c>
+      <c r="N2" s="6">
+        <v>957.26949999999999</v>
+      </c>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7">
+        <v>891.56219999999996</v>
+      </c>
+      <c r="Q2" s="6">
+        <f>MIN(N2:P2)</f>
+        <v>891.56219999999996</v>
+      </c>
+      <c r="R2" s="7">
+        <f>MAX(N2:P2)</f>
+        <v>957.26949999999999</v>
+      </c>
+      <c r="S2" s="8">
+        <f>AVERAGE(N2:P2)</f>
+        <v>924.41584999999998</v>
+      </c>
+      <c r="U2" s="3">
+        <f>(S2-C2)/C2</f>
+        <v>0.39851111951588497</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>661</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1000</v>
+      </c>
+      <c r="F3" s="5">
+        <f t="shared" ref="F3:F5" si="0">E3* 0.3</f>
+        <v>300</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="12">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <f t="shared" ref="I3:I6" si="1">E3*0.3 -H3</f>
+        <v>300</v>
+      </c>
+      <c r="J3" s="5">
+        <f t="shared" ref="J3:J5" si="2">E3*0.4</f>
+        <v>400</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="5">
+        <f t="shared" ref="L3:L6" si="3">F3+H3+I3+J3</f>
+        <v>1000</v>
+      </c>
+      <c r="N3" s="9">
+        <v>1224.1606999999999</v>
+      </c>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10">
+        <v>1265.5310999999999</v>
+      </c>
+      <c r="Q3" s="9">
+        <f t="shared" ref="Q3:Q6" si="4">MIN(N3:P3)</f>
+        <v>1224.1606999999999</v>
+      </c>
+      <c r="R3" s="10">
+        <f t="shared" ref="R3:R6" si="5">MAX(N3:P3)</f>
+        <v>1265.5310999999999</v>
+      </c>
+      <c r="S3" s="11">
+        <f t="shared" ref="S3:S6" si="6">AVERAGE(N3:P3)</f>
+        <v>1244.8458999999998</v>
+      </c>
+      <c r="U3" s="3">
+        <f t="shared" ref="U3:U8" si="7">(S3-C3)/C3</f>
+        <v>0.88327670196671682</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>661</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="E4" s="13">
+        <v>100</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="5">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="N4" s="9">
+        <v>903.66309999999999</v>
+      </c>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10">
+        <v>921.55870000000004</v>
+      </c>
+      <c r="Q4" s="9">
+        <f t="shared" si="4"/>
+        <v>903.66309999999999</v>
+      </c>
+      <c r="R4" s="10">
+        <f t="shared" si="5"/>
+        <v>921.55870000000004</v>
+      </c>
+      <c r="S4" s="11">
+        <f t="shared" si="6"/>
+        <v>912.61090000000002</v>
+      </c>
+      <c r="U4" s="3">
+        <f t="shared" si="7"/>
+        <v>0.38065189107413011</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>661</v>
+      </c>
+      <c r="D5">
+        <v>50</v>
+      </c>
+      <c r="E5" s="13">
+        <v>10000</v>
+      </c>
+      <c r="F5" s="5">
+        <f t="shared" si="0"/>
+        <v>3000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5">
+        <f t="shared" si="1"/>
+        <v>2999</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" si="2"/>
+        <v>4000</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="5">
+        <f t="shared" si="3"/>
+        <v>10000</v>
+      </c>
+      <c r="N5" s="9">
+        <v>883.24</v>
+      </c>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10">
+        <v>923.11810000000003</v>
+      </c>
+      <c r="Q5" s="9">
+        <f t="shared" si="4"/>
+        <v>883.24</v>
+      </c>
+      <c r="R5" s="10">
+        <f t="shared" si="5"/>
+        <v>923.11810000000003</v>
+      </c>
+      <c r="S5" s="11">
+        <f t="shared" si="6"/>
+        <v>903.17904999999996</v>
+      </c>
+      <c r="U5" s="3">
+        <f t="shared" si="7"/>
+        <v>0.36638282904689856</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>661</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1000</v>
+      </c>
+      <c r="F6" s="5">
+        <f>E6* 0.5</f>
+        <v>500</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" si="1"/>
+        <v>299</v>
+      </c>
+      <c r="J6" s="14">
+        <f>E6*0.2</f>
+        <v>200</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="5">
+        <f t="shared" si="3"/>
+        <v>1000</v>
+      </c>
+      <c r="N6" s="9">
+        <v>944.18290000000002</v>
+      </c>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10">
+        <v>999.06479999999999</v>
+      </c>
+      <c r="Q6" s="9">
+        <f t="shared" si="4"/>
+        <v>944.18290000000002</v>
+      </c>
+      <c r="R6" s="10">
+        <f t="shared" si="5"/>
+        <v>999.06479999999999</v>
+      </c>
+      <c r="S6" s="11">
+        <f t="shared" si="6"/>
+        <v>971.62384999999995</v>
+      </c>
+      <c r="U6" s="3">
+        <f t="shared" si="7"/>
+        <v>0.46993018154311639</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>661</v>
+      </c>
+      <c r="D7">
+        <v>50</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1000</v>
+      </c>
+      <c r="F7" s="5">
+        <f>E7* 0.3</f>
+        <v>300</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5">
+        <f>E7*0.3 -H7</f>
+        <v>299</v>
+      </c>
+      <c r="J7" s="5">
+        <f>E7*0.4</f>
+        <v>400</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="5">
+        <f t="shared" ref="L7" si="8">F7+H7+I7+J7</f>
+        <v>1000</v>
+      </c>
+      <c r="N7" s="9"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="9">
+        <f t="shared" ref="Q7:Q8" si="9">MIN(N7:P7)</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="10">
+        <f t="shared" ref="R7:R8" si="10">MAX(N7:P7)</f>
+        <v>0</v>
+      </c>
+      <c r="S7" s="11" t="e">
+        <f t="shared" ref="S7:S8" si="11">AVERAGE(N7:P7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U7" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>661</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1000</v>
+      </c>
+      <c r="F8" s="5">
+        <f>E8* 0.3</f>
+        <v>300</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5">
+        <f>E8*0.1 -H8</f>
+        <v>99</v>
+      </c>
+      <c r="J8" s="5">
+        <f>E8*0.6</f>
+        <v>600</v>
+      </c>
+      <c r="K8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="5">
+        <f t="shared" ref="L8" si="12">F8+H8+I8+J8</f>
+        <v>1000</v>
+      </c>
+      <c r="N8" s="15">
+        <v>877.87</v>
+      </c>
+      <c r="P8" s="16">
+        <v>873.77239999999995</v>
+      </c>
+      <c r="Q8" s="15">
+        <f t="shared" si="9"/>
+        <v>873.77239999999995</v>
+      </c>
+      <c r="R8" s="17">
+        <f t="shared" si="10"/>
+        <v>877.87</v>
+      </c>
+      <c r="S8" s="16">
+        <f t="shared" si="11"/>
+        <v>875.82119999999998</v>
+      </c>
+      <c r="U8" s="3">
+        <f t="shared" si="7"/>
+        <v>0.32499425113464442</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>661</v>
+      </c>
+      <c r="D17">
+        <v>10000</v>
+      </c>
+      <c r="E17">
+        <v>10000</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ref="F17:F20" si="13">E17/2</f>
+        <v>5000</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ref="I17:I20" si="14">E17*0.4 -H17</f>
+        <v>4000</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ref="J17:J20" si="15">E17*0.1</f>
+        <v>1000</v>
+      </c>
+      <c r="K17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ref="L17:L20" si="16">F17+H17+I17+J17</f>
+        <v>10000</v>
+      </c>
+      <c r="U17" s="3">
+        <f>(Q17-C17)/C17</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>211</v>
+      </c>
+      <c r="D18">
+        <v>10000</v>
+      </c>
+      <c r="E18">
+        <v>1000</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="13"/>
+        <v>500</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="14"/>
+        <v>400</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="15"/>
+        <v>100</v>
+      </c>
+      <c r="K18" t="s">
+        <v>15</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="16"/>
+        <v>1000</v>
+      </c>
+      <c r="U18" s="3">
+        <f>(Q18-C18)/C18</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>805</v>
+      </c>
+      <c r="D19">
+        <v>10000</v>
+      </c>
+      <c r="E19">
+        <v>1000</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="13"/>
+        <v>500</v>
+      </c>
+      <c r="G19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="14"/>
+        <v>399</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="15"/>
+        <v>100</v>
+      </c>
+      <c r="K19" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="16"/>
+        <v>1000</v>
+      </c>
+      <c r="U19" s="3">
+        <f t="shared" ref="U19:U20" si="17">(Q19-C19)/C19</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20">
+        <v>1764</v>
+      </c>
+      <c r="D20">
+        <v>10000</v>
+      </c>
+      <c r="E20">
+        <v>10000</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="13"/>
+        <v>5000</v>
+      </c>
+      <c r="G20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="14"/>
+        <v>4000</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="15"/>
+        <v>1000</v>
+      </c>
+      <c r="K20" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="16"/>
+        <v>10000</v>
+      </c>
+      <c r="U20" s="3">
+        <f t="shared" si="17"/>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>